<commit_message>
Fixed code, successfully consolidated attendance
</commit_message>
<xml_diff>
--- a/consolidated_attendance.xlsx
+++ b/consolidated_attendance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Full Name</t>
   </si>
@@ -25,58 +25,45 @@
     <t>Card ID Number</t>
   </si>
   <si>
-    <t>Digital Tech x Sustainability  with Alibaba Cloud_x</t>
-  </si>
-  <si>
-    <t>Digital Tech x Sustainability  with Alibaba Cloud_y</t>
-  </si>
-  <si>
     <t>Digital Tech x Sustainability  with Alibaba Cloud</t>
   </si>
   <si>
     <t>Azbil Event</t>
   </si>
   <si>
-    <t>0       John
-1      Alice
-2    Charlie
-3      Diana
-4       Emma
-Name: First Name, dtype: object 0         Doe
-1     Johnson
-2    Williams
-3      Miller
-4       Davis
-Name: Last Name, dtype: object</t>
-  </si>
-  <si>
-    <t>0     John
-1     Jane
-2    Alice
-3      Bob
-Name: First Name, dtype: object 0        Doe
-1      Smith
-2    Johnson
-3      Brown
-Name: Last Name, dtype: object</t>
-  </si>
-  <si>
-    <t>0   NaN
-1   NaN
-2   NaN
-3   NaN
-4   NaN
-Name: First Name, dtype: float64 0   NaN
-1   NaN
-2   NaN
-3   NaN
-4   NaN
-Name: Last Name, dtype: float64</t>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>Alice Johnson</t>
+  </si>
+  <si>
+    <t>Bob Brown</t>
+  </si>
+  <si>
+    <t>Charlie Williams</t>
+  </si>
+  <si>
+    <t>Diana Miller</t>
+  </si>
+  <si>
+    <t>Emma Davis</t>
+  </si>
+  <si>
+    <t>john.doe@campus.edu</t>
+  </si>
+  <si>
+    <t>jane.smith@campus.edu</t>
   </si>
   <si>
     <t>alice.j@campus.edu</t>
   </si>
   <si>
+    <t>bob.b@campus.edu</t>
+  </si>
+  <si>
     <t>charlie.w@campus.edu</t>
   </si>
   <si>
@@ -86,21 +73,18 @@
     <t>emma.d@campus.edu</t>
   </si>
   <si>
-    <t>john.doe@campus.edu</t>
-  </si>
-  <si>
-    <t>bob.b@campus.edu</t>
-  </si>
-  <si>
-    <t>jane.smith@campus.edu</t>
-  </si>
-  <si>
-    <t>nan</t>
+    <t>A1234567B</t>
+  </si>
+  <si>
+    <t>A2345678C</t>
   </si>
   <si>
     <t>A3456789D</t>
   </si>
   <si>
+    <t>A4567890E</t>
+  </si>
+  <si>
     <t>A5678901F</t>
   </si>
   <si>
@@ -108,15 +92,6 @@
   </si>
   <si>
     <t>A7890123H</t>
-  </si>
-  <si>
-    <t>A1234567B</t>
-  </si>
-  <si>
-    <t>A4567890E</t>
-  </si>
-  <si>
-    <t>A2345678C</t>
   </si>
 </sst>
 </file>
@@ -474,13 +449,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,261 +471,124 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
+      <c r="E8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>